<commit_message>
revise hw3 of DS
</commit_message>
<xml_diff>
--- a/DataStructure_HW/HW3/hw3_OriginalData_diagram.xlsx
+++ b/DataStructure_HW/HW3/hw3_OriginalData_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywt01\Documents\codes\nccu_cs_hw\DataStructure_HW\HW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5463B1-4A05-489E-8E03-CC614033B056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBDC815-6524-4963-83DB-B562F5FC5534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insert_t" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>y = 0.0044*x^0.2702</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>hash table</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -89,6 +85,10 @@
   </si>
   <si>
     <t>y = 0.0003*x^0.4769</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>y = 0.0901*x^0.0171</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -5315,36 +5315,6 @@
                   <c:y val="-0.24077317214619243"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="zh-TW" sz="1200" baseline="0"/>
-                      <a:t>y = 0.0003x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="zh-TW" sz="1200" baseline="30000"/>
-                      <a:t>0.4769</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1200"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5949,6 +5919,86 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.822437579917895E-2"/>
+                  <c:y val="0.10009458384900065"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="zh-TW" altLang="en-US" sz="1200" baseline="0"/>
+                      <a:t>y = 0.0901x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="zh-TW" altLang="en-US" sz="1200" baseline="30000"/>
+                      <a:t>0.0171</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1200"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-TW"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>search_t!$B$2:$B$22</c:f>
@@ -6739,13 +6789,13 @@
                   <c:v>0.26492399999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.3581727135280473</c:v>
+                  <c:v>0.37289726507689397</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.43776464197228271</c:v>
+                  <c:v>0.45772408782409374</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.53504321943864108</c:v>
+                  <c:v>0.5618473509887395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6758,137 +6808,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>search_t!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>search_t!$B$2:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>524288</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2097152</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4194304</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8388608</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16777216</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>33554432</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>67108864</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>134217728</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>268435456</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>536870912</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1073741824</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>search_t!#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E7F8-43E0-A272-6EAFF96D6C8E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>search_t!$E$1</c:f>
@@ -7039,31 +6960,31 @@
                   <c:v>0.44289699999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18732951402033471</c:v>
+                  <c:v>0.43198410114980518</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.23567164923088568</c:v>
+                  <c:v>0.60121383810177031</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.29648892509899194</c:v>
+                  <c:v>0.8367393109213368</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.37300066848615848</c:v>
+                  <c:v>1.1645318688133723</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.46925698369565794</c:v>
+                  <c:v>1.6207371349491404</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.59035314237062508</c:v>
+                  <c:v>2.2556607774759976</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.74269929871284646</c:v>
+                  <c:v>3.1393157060002066</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.93435980723933787</c:v>
+                  <c:v>4.3691423818466788</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1754801046632948</c:v>
+                  <c:v>6.0807535592431883</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7077,7 +6998,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>search_t!$F$1</c:f>
@@ -7240,19 +7161,19 @@
                   <c:v>0.12118</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.57312400894348636</c:v>
+                  <c:v>0.12262039958939788</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.69117322653499713</c:v>
+                  <c:v>0.12408244427730211</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.83353763168889461</c:v>
+                  <c:v>0.12556192142078945</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0052255451569512</c:v>
+                  <c:v>0.12705903887295103</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2122768765564689</c:v>
+                  <c:v>0.12857400696518087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7577,7 +7498,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="zh-TW" altLang="en-US" sz="1800"/>
-              <a:t>圖六</a:t>
+              <a:t>圖五</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7977,13 +7898,13 @@
                   <c:v>0.26492399999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.3581727135280473</c:v>
+                  <c:v>0.37289726507689397</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.43776464197228271</c:v>
+                  <c:v>0.45772408782409374</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.53504321943864108</c:v>
+                  <c:v>0.5618473509887395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7996,197 +7917,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>search_t!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Skip List_0.5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>search_t!$B$2:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>524288</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2097152</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4194304</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8388608</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16777216</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>33554432</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>67108864</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>134217728</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>268435456</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>536870912</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1073741824</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>search_t!$E$2:$E$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>1.1863E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5159000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7902000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1901E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.7376000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1778000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.5465E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.3954000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.152943</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.10773099999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.41801899999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.44289699999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.18732951402033471</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.23567164923088568</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.29648892509899194</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.37300066848615848</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.46925698369565794</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.59035314237062508</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.74269929871284646</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.93435980723933787</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.1754801046632948</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-AC86-43F8-A2C0-E5E119B7628B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>search_t!$F$1</c:f>
@@ -8349,19 +8081,19 @@
                   <c:v>0.12118</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.57312400894348636</c:v>
+                  <c:v>0.12262039958939788</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.69117322653499713</c:v>
+                  <c:v>0.12408244427730211</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.83353763168889461</c:v>
+                  <c:v>0.12556192142078945</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0052255451569512</c:v>
+                  <c:v>0.12705903887295103</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2122768765564689</c:v>
+                  <c:v>0.12857400696518087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8387,21 +8119,21 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="2"/>
+                <c:idx val="3"/>
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>search_t!#REF!</c15:sqref>
+                          <c15:sqref>search_t!$E$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>#REF!</c:v>
+                        <c:v>Skip List_0.5</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -8409,7 +8141,7 @@
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent3"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -8420,11 +8152,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent3"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent3"/>
+                        <a:schemeClr val="accent4"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -8513,15 +8245,75 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>search_t!#REF!</c15:sqref>
+                          <c15:sqref>search_t!$E$2:$E$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="1"/>
+                      <c:ptCount val="21"/>
                       <c:pt idx="0">
-                        <c:v>1</c:v>
+                        <c:v>1.1863E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.5159000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.7902000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2.1901E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2.7376000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3.1778000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5.5465E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5.3954000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.152943</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.10773099999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.41801899999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.44289699999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.43198410114980518</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.60121383810177031</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.8367393109213368</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>1.1645318688133723</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.6207371349491404</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2.2556607774759976</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>3.1393157060002066</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>4.3691423818466788</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>6.0807535592431883</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -8529,7 +8321,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-AC86-43F8-A2C0-E5E119B7628B}"/>
+                    <c16:uniqueId val="{00000003-AC86-43F8-A2C0-E5E119B7628B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -14258,8 +14050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -14290,7 +14082,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -14769,16 +14561,16 @@
         <v>3</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -14793,8 +14585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737C9493-ED4E-44AB-B916-0A25225F2F82}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -14822,7 +14614,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -15096,8 +14888,8 @@
         <v>0.129325</v>
       </c>
       <c r="E14" s="9">
-        <f t="shared" ref="E14:E22" si="2" xml:space="preserve"> 0.0012*B14^0.3312</f>
-        <v>0.18732951402033471</v>
+        <f xml:space="preserve">  0.0003*B14^0.4769</f>
+        <v>0.43198410114980518</v>
       </c>
       <c r="F14" s="8">
         <v>0.116156</v>
@@ -15119,8 +14911,8 @@
         <v>0.139935</v>
       </c>
       <c r="E15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.23567164923088568</v>
+        <f t="shared" ref="E15:E22" si="2" xml:space="preserve">  0.0003*B15^0.4769</f>
+        <v>0.60121383810177031</v>
       </c>
       <c r="F15" s="8">
         <v>0.115837</v>
@@ -15143,7 +14935,7 @@
       </c>
       <c r="E16" s="9">
         <f t="shared" si="2"/>
-        <v>0.29648892509899194</v>
+        <v>0.8367393109213368</v>
       </c>
       <c r="F16" s="8">
         <v>0.116533</v>
@@ -15166,7 +14958,7 @@
       </c>
       <c r="E17" s="9">
         <f t="shared" si="2"/>
-        <v>0.37300066848615848</v>
+        <v>1.1645318688133723</v>
       </c>
       <c r="F17" s="8">
         <v>0.12118</v>
@@ -15189,11 +14981,11 @@
       </c>
       <c r="E18" s="9">
         <f t="shared" si="2"/>
-        <v>0.46925698369565794</v>
+        <v>1.6207371349491404</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" ref="F12:F22" si="3" xml:space="preserve"> 0.0044*B18^0.2702</f>
-        <v>0.57312400894348636</v>
+        <f xml:space="preserve"> 0.0901*B18^0.0171</f>
+        <v>0.12262039958939788</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -15213,11 +15005,11 @@
       </c>
       <c r="E19" s="9">
         <f t="shared" si="2"/>
-        <v>0.59035314237062508</v>
+        <v>2.2556607774759976</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="3"/>
-        <v>0.69117322653499713</v>
+        <f t="shared" ref="F19:F22" si="3" xml:space="preserve"> 0.0901*B19^0.0171</f>
+        <v>0.12408244427730211</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -15233,16 +15025,16 @@
         <v>7.9192793519881705E-2</v>
       </c>
       <c r="D20" s="9">
-        <f t="shared" ref="D20:D22" si="4" xml:space="preserve"> 0.0013*B20^0.2895</f>
-        <v>0.3581727135280473</v>
+        <f xml:space="preserve"> 0.0012*B20^0.2957</f>
+        <v>0.37289726507689397</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="2"/>
-        <v>0.74269929871284646</v>
+        <v>3.1393157060002066</v>
       </c>
       <c r="F20" s="9">
         <f t="shared" si="3"/>
-        <v>0.83353763168889461</v>
+        <v>0.12556192142078945</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -15258,16 +15050,16 @@
         <v>8.5206834353683189E-2</v>
       </c>
       <c r="D21" s="9">
-        <f t="shared" si="4"/>
-        <v>0.43776464197228271</v>
+        <f t="shared" ref="D21:D22" si="4" xml:space="preserve"> 0.0012*B21^0.2957</f>
+        <v>0.45772408782409374</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="2"/>
-        <v>0.93435980723933787</v>
+        <v>4.3691423818466788</v>
       </c>
       <c r="F21" s="9">
         <f t="shared" si="3"/>
-        <v>1.0052255451569512</v>
+        <v>0.12705903887295103</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -15284,15 +15076,15 @@
       </c>
       <c r="D22" s="9">
         <f t="shared" si="4"/>
-        <v>0.53504321943864108</v>
+        <v>0.5618473509887395</v>
       </c>
       <c r="E22" s="9">
         <f t="shared" si="2"/>
-        <v>1.1754801046632948</v>
+        <v>6.0807535592431883</v>
       </c>
       <c r="F22" s="9">
         <f t="shared" si="3"/>
-        <v>1.2122768765564689</v>
+        <v>0.12857400696518087</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -15301,21 +15093,22 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>